<commit_message>
Excel data failure fix
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTestDataFiles/SecurityAdminTestData.xlsx
+++ b/src/test/resources/ExcelTestDataFiles/SecurityAdminTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SignetAutomation\SampleSeleniumTestNGProject\src\test\resources\ExcelTestDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16948B8F-1029-4D90-98D4-0ADA47EC5ABA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BEB8ED-59D2-41F4-AEC0-C3B750F0C091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -213,15 +213,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -506,52 +507,53 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="42" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="43" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -666,158 +668,158 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>1234</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="5" t="b">
+      <c r="H6" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6">
         <v>654</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="5" t="b">
+      <c r="H7" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6">
         <v>879</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="5" t="b">
+      <c r="H8" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6">
         <v>568</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="5" t="b">
+      <c r="H9" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>